<commit_message>
Diagras de caso de Uso
</commit_message>
<xml_diff>
--- a/Documents/Reglas de negocio.xlsx
+++ b/Documents/Reglas de negocio.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ff47571d30268be/Documentos/6/APLICACIONE II/Proyecto/SIGDCOLTA/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{119855CD-966E-4232-8FE4-29E61D867C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B505015C-A221-4013-80D9-BD6A08B03E88}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{119855CD-966E-4232-8FE4-29E61D867C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92188ACC-7AB0-4AED-A592-47E841BBC410}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="868" xr2:uid="{80B57F57-6BCE-48EE-8981-A0776E67AA93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="868" activeTab="2" xr2:uid="{80B57F57-6BCE-48EE-8981-A0776E67AA93}"/>
   </bookViews>
   <sheets>
-    <sheet name="Asignacion de roles" sheetId="2" r:id="rId1"/>
-    <sheet name="Registo y Consulta de Asistenci" sheetId="3" r:id="rId2"/>
-    <sheet name="Consultar Dias" sheetId="4" r:id="rId3"/>
-    <sheet name="Mostrar Contenido Rol" sheetId="5" r:id="rId4"/>
-    <sheet name="CRUD" sheetId="6" r:id="rId5"/>
-    <sheet name="Login" sheetId="7" r:id="rId6"/>
-    <sheet name="Registro Contratacion" sheetId="8" r:id="rId7"/>
-    <sheet name="Generar solicitudes" sheetId="1" r:id="rId8"/>
+    <sheet name="Login" sheetId="7" r:id="rId1"/>
+    <sheet name="Asignacion de roles" sheetId="2" r:id="rId2"/>
+    <sheet name="Registo y Consulta de Asistenci" sheetId="3" r:id="rId3"/>
+    <sheet name="Consultar Dias" sheetId="4" r:id="rId4"/>
+    <sheet name="Generar solicitudes" sheetId="1" r:id="rId5"/>
+    <sheet name="Mostrar Contenido Rol" sheetId="5" r:id="rId6"/>
+    <sheet name="CRUD" sheetId="6" r:id="rId7"/>
+    <sheet name="Registro Contratacion" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1318,9 +1318,6 @@
     <t>Mostrar mensaje de error notificando que ya existe un registro de asistencia para el mismo empleado en la misma fecha y hora.</t>
   </si>
   <si>
-    <t>as credenciales proporcionadas durante el inicio de sesión deben ser válidas y correspondientes a un usuario autorizado como ERH</t>
-  </si>
-  <si>
     <t>Mostrar mensaje de error si las credenciales no son válidas o si el usuario no tiene permisos de ERH.</t>
   </si>
   <si>
@@ -1403,6 +1400,9 @@
   </si>
   <si>
     <t>Mostrar mensaje de error si la cuenta del usuario está bloqueada, asegurando la seguridad antes de realizar cambios de rol.</t>
+  </si>
+  <si>
+    <t>Las credenciales proporcionadas durante el inicio de sesión deben ser válidas y correspondientes a un usuario autorizado como ERH</t>
   </si>
 </sst>
 </file>
@@ -1622,24 +1622,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1653,9 +1635,46 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1665,39 +1684,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2012,10 +2012,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A455E2C9-027A-4714-A75D-E5241D0081E8}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="39.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="74" style="2" customWidth="1"/>
+    <col min="4" max="4" width="131.7109375" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A2" s="24"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A3" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A4" s="43"/>
+      <c r="B4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A5" s="43"/>
+      <c r="B5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A6" s="43"/>
+      <c r="B6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A7" s="43"/>
+      <c r="B7" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A8" s="43"/>
+      <c r="B8" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A9" s="43"/>
+      <c r="B9" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A10" s="44"/>
+      <c r="B10" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:4" s="22" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A12" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A13" s="43"/>
+      <c r="B13" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A14" s="43"/>
+      <c r="B14" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A15" s="43"/>
+      <c r="B15" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A16" s="43"/>
+      <c r="B16" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A17" s="43"/>
+      <c r="B17" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A18" s="44"/>
+      <c r="B18" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A12:A18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AD3F6A-B73B-468C-8ED7-269B49C2CF96}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+    <sheetView zoomScale="66" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2043,211 +2263,211 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="60.75" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>433</v>
       </c>
-      <c r="D2" s="44" t="s">
-        <v>434</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="57" customHeight="1">
-      <c r="A3" s="38"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>435</v>
+        <v>430</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="48" customHeight="1">
-      <c r="A4" s="38"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="D4" s="44" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="5" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A5" s="38"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>438</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>439</v>
-      </c>
     </row>
     <row r="6" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A6" s="38"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="44"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A7" s="38"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="44"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A8" s="38"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="44"/>
+      <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" s="14" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A9" s="45"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="45"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10" s="31" t="s">
         <v>433</v>
       </c>
-      <c r="D10" s="44" t="s">
-        <v>434</v>
-      </c>
     </row>
     <row r="11" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A11" s="38"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>435</v>
+        <v>430</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A12" s="38"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D12" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="D12" s="44" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="13" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A13" s="38"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>438</v>
       </c>
-      <c r="D13" s="44" t="s">
-        <v>439</v>
-      </c>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A14" s="45"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="45"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:4" s="15" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>440</v>
       </c>
-      <c r="D15" s="48" t="s">
-        <v>441</v>
-      </c>
     </row>
     <row r="16" spans="1:4" s="15" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A16" s="47"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" s="34" t="s">
         <v>442</v>
       </c>
-      <c r="D16" s="48" t="s">
-        <v>443</v>
-      </c>
     </row>
     <row r="17" spans="1:4" s="15" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A17" s="47"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>444</v>
       </c>
-      <c r="D17" s="48" t="s">
-        <v>445</v>
-      </c>
     </row>
     <row r="18" spans="1:4" s="15" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A18" s="47"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="35" t="s">
+        <v>445</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>446</v>
       </c>
-      <c r="D18" s="48" t="s">
-        <v>447</v>
-      </c>
     </row>
     <row r="19" spans="1:4" s="15" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A19" s="47"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="49" t="s">
-        <v>432</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>448</v>
+      <c r="C19" s="35" t="s">
+        <v>431</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="15" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A20" s="47"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="48"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="34"/>
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A21" s="45"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="45"/>
+      <c r="D21" s="32"/>
     </row>
     <row r="22" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="36" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2256,91 +2476,91 @@
       <c r="C22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="44" t="s">
-        <v>449</v>
+      <c r="D22" s="31" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A23" s="38"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>450</v>
+      <c r="D23" s="31" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A24" s="38"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="44" t="s">
-        <v>451</v>
+      <c r="D24" s="31" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A25" s="38"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="D25" s="31" t="s">
         <v>452</v>
       </c>
-      <c r="D25" s="44" t="s">
-        <v>453</v>
-      </c>
     </row>
     <row r="26" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A26" s="38"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="44"/>
+      <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A27" s="38"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="44"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A28" s="38"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="44"/>
+      <c r="D28" s="31"/>
     </row>
     <row r="29" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A29" s="38"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="44"/>
+      <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A30" s="38"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="44"/>
+      <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4" s="14" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A31" s="45"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="45"/>
+      <c r="D31" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2354,12 +2574,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD7A112-304A-4361-9BE2-CCAB4746A598}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="35.25" customHeight="1"/>
@@ -2386,516 +2606,516 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="31" t="s">
+        <v>453</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="D2" s="44" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A3" s="39"/>
+      <c r="B3" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="44" t="s">
+      <c r="D3" s="31" t="s">
         <v>427</v>
       </c>
-      <c r="D3" s="44" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A4" s="39"/>
+      <c r="B4" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="44" t="s">
+      <c r="D4" s="31" t="s">
         <v>429</v>
       </c>
-      <c r="D4" s="44" t="s">
-        <v>430</v>
-      </c>
     </row>
     <row r="5" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="44" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="44" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-    </row>
-    <row r="10" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="44" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-    </row>
-    <row r="11" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="44" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+    </row>
+    <row r="11" spans="1:4" ht="50.25" customHeight="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="44" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A13" s="34"/>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="40"/>
+      <c r="B13" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A14" s="43"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="31" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="44" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A17" s="34"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A18" s="43"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
     </row>
     <row r="19" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="31" t="s">
         <v>409</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="31" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44" t="s">
+      <c r="A20" s="39"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31" t="s">
         <v>411</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="31" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="44" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="31" t="s">
         <v>413</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="31" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="44" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="33" t="s">
         <v>415</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="31" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31" t="s">
         <v>417</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="31" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="44" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="31" t="s">
         <v>419</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="31" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="44" t="s">
+      <c r="A25" s="39"/>
+      <c r="B25" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="31" t="s">
         <v>421</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="31" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="31" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="14" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A27" s="43"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="31" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="44" t="s">
+      <c r="A29" s="39"/>
+      <c r="B29" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="44" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
     </row>
     <row r="31" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="44" t="s">
+      <c r="A31" s="39"/>
+      <c r="B31" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
     </row>
     <row r="32" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="44" t="s">
+      <c r="A32" s="40"/>
+      <c r="B32" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4" s="14" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A33" s="43"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
     </row>
     <row r="34" spans="1:4" ht="45.75" customHeight="1">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="31" t="s">
         <v>403</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="31" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A35" s="26"/>
-      <c r="B35" s="44" t="s">
+      <c r="A35" s="39"/>
+      <c r="B35" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="31" t="s">
         <v>405</v>
       </c>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="31" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A36" s="26"/>
-      <c r="B36" s="44" t="s">
+      <c r="A36" s="39"/>
+      <c r="B36" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="31" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="44" t="s">
+      <c r="A37" s="39"/>
+      <c r="B37" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A38" s="26"/>
-      <c r="B38" s="44" t="s">
+      <c r="A38" s="39"/>
+      <c r="B38" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
     </row>
     <row r="39" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A39" s="26"/>
-      <c r="B39" s="44" t="s">
+      <c r="A39" s="39"/>
+      <c r="B39" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
     </row>
     <row r="40" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A40" s="26"/>
-      <c r="B40" s="44" t="s">
+      <c r="A40" s="39"/>
+      <c r="B40" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
     </row>
     <row r="41" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="44" t="s">
+      <c r="A41" s="40"/>
+      <c r="B41" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
     </row>
     <row r="42" spans="1:4" s="14" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A42" s="43"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
     </row>
     <row r="43" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="31" t="s">
         <v>398</v>
       </c>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="31" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="44" t="s">
+      <c r="A44" s="39"/>
+      <c r="B44" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="31" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="44" t="s">
+      <c r="A45" s="39"/>
+      <c r="B45" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="44" t="s">
+      <c r="D45" s="31" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A46" s="26"/>
-      <c r="B46" s="44" t="s">
+      <c r="A46" s="39"/>
+      <c r="B46" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="44" t="s">
+      <c r="C46" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="31" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A47" s="34"/>
-      <c r="B47" s="44" t="s">
+      <c r="A47" s="40"/>
+      <c r="B47" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
     </row>
     <row r="48" spans="1:4" s="14" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A48" s="43"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
     </row>
     <row r="49" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="44" t="s">
+      <c r="C49" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="44" t="s">
+      <c r="D49" s="31" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="44" t="s">
+      <c r="A50" s="39"/>
+      <c r="B50" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
     </row>
     <row r="51" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A51" s="26"/>
-      <c r="B51" s="44" t="s">
+      <c r="A51" s="39"/>
+      <c r="B51" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
     </row>
     <row r="52" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A52" s="26"/>
-      <c r="B52" s="44" t="s">
+      <c r="A52" s="39"/>
+      <c r="B52" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
     </row>
     <row r="53" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="44" t="s">
+      <c r="A53" s="39"/>
+      <c r="B53" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A54" s="26"/>
-      <c r="B54" s="44" t="s">
+      <c r="A54" s="39"/>
+      <c r="B54" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A55" s="34"/>
-      <c r="B55" s="44" t="s">
+      <c r="A55" s="40"/>
+      <c r="B55" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2912,11 +3132,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5494A7-E0F5-4F3E-B3AA-2CD83B32EE1A}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="78" workbookViewId="0">
+    <sheetView zoomScale="78" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2943,248 +3163,248 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="38" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="31" t="s">
         <v>366</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="31" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A3" s="26"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="31" t="s">
         <v>369</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="31" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A4" s="26"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="31" t="s">
         <v>371</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="31" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A5" s="26"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="31" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="31" t="s">
         <v>375</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="31" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A7" s="26"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A8" s="34"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" s="14" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A9" s="43"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="38" t="s">
         <v>124</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="31" t="s">
         <v>377</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="31" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A11" s="26"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="31" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A12" s="26"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="31" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A13" s="26"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="31" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A14" s="26"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="31" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A15" s="26"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="31" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A16" s="26"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="31" t="s">
         <v>388</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="31" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A17" s="26"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A18" s="26"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
     </row>
     <row r="19" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A19" s="34"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A20" s="43"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
     </row>
     <row r="21" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="38" t="s">
         <v>123</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="31" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A22" s="26"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="31" t="s">
         <v>391</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="31" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A23" s="26"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="31" t="s">
         <v>393</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="31" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="55.5" customHeight="1">
-      <c r="A24" s="34"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="31" t="s">
         <v>395</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="31" t="s">
         <v>396</v>
       </c>
     </row>
@@ -3198,7 +3418,255 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9559937-0F27-4DE2-A20B-39F6C6177D47}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="30.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="103.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A3" s="49"/>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A4" s="49"/>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A5" s="49"/>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A6" s="49"/>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A8" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A9" s="46"/>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A10" s="46"/>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A11" s="46"/>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="11"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A13" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" customHeight="1">
+      <c r="A14" s="47"/>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A15" s="47"/>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A16" s="47"/>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A17" s="47"/>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A19" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A20" s="36"/>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A21" s="36"/>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A2:A6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11AE6C1-E673-49C8-BFF3-EE20E624F7EF}">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -3230,7 +3698,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="38" t="s">
         <v>145</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3244,7 +3712,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A3" s="26"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="3" t="s">
         <v>149</v>
       </c>
@@ -3256,7 +3724,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A4" s="26"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="3" t="s">
         <v>150</v>
       </c>
@@ -3268,7 +3736,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A5" s="26"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="3" t="s">
         <v>151</v>
       </c>
@@ -3280,7 +3748,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="3" t="s">
         <v>152</v>
       </c>
@@ -3292,7 +3760,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A7" s="26"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="3" t="s">
         <v>153</v>
       </c>
@@ -3304,7 +3772,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A8" s="34"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="3" t="s">
         <v>154</v>
       </c>
@@ -3312,13 +3780,13 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A9" s="43"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>146</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -3332,7 +3800,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A11" s="42"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="3" t="s">
         <v>162</v>
       </c>
@@ -3344,7 +3812,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A12" s="42"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="3" t="s">
         <v>163</v>
       </c>
@@ -3356,7 +3824,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A13" s="42"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="3" t="s">
         <v>164</v>
       </c>
@@ -3364,7 +3832,7 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A14" s="42"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="3" t="s">
         <v>158</v>
       </c>
@@ -3372,7 +3840,7 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="3" t="s">
         <v>159</v>
       </c>
@@ -3380,7 +3848,7 @@
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A16" s="42"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="3" t="s">
         <v>160</v>
       </c>
@@ -3388,7 +3856,7 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A17" s="42"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="3" t="s">
         <v>161</v>
       </c>
@@ -3409,7 +3877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE906BB1-52BF-4605-B1B4-F117164F9EE5}">
   <dimension ref="A1:D55"/>
   <sheetViews>
@@ -3441,372 +3909,372 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="25" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="25" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="25" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="25" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="25" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="31" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="25" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="31" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="25" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="25" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A12" s="34"/>
-      <c r="B12" s="31" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="25" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="25" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="25" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="25" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="25" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A19" s="34"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="25" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="49.5" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="25" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="31" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="25" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="25" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="31" t="s">
+      <c r="A25" s="39"/>
+      <c r="B25" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="25" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="41.25" customHeight="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25" t="s">
         <v>338</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="25" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="18" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="25" t="s">
         <v>358</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="25" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="31" t="s">
+      <c r="A29" s="39"/>
+      <c r="B29" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="25" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="25" t="s">
         <v>361</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="25" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="31" t="s">
+      <c r="A31" s="39"/>
+      <c r="B31" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="25" t="s">
         <v>355</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="25" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="31" t="s">
+      <c r="A32" s="39"/>
+      <c r="B32" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="25" t="s">
         <v>356</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="25" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="31" t="s">
+      <c r="A33" s="39"/>
+      <c r="B33" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="25" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="31" t="s">
+      <c r="A34" s="39"/>
+      <c r="B34" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
     </row>
     <row r="35" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="40"/>
+      <c r="B35" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
     </row>
     <row r="55" spans="1:1" ht="35.25" customHeight="1">
       <c r="A55" s="17" t="s">
@@ -3825,227 +4293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A455E2C9-027A-4714-A75D-E5241D0081E8}">
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="39.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="29.5703125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="80.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="74" style="2" customWidth="1"/>
-    <col min="4" max="4" width="131.7109375" style="21" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="21"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A1" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="30"/>
-    </row>
-    <row r="3" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A3" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A7" s="36"/>
-      <c r="B7" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A8" s="36"/>
-      <c r="B8" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A9" s="36"/>
-      <c r="B9" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A10" s="37"/>
-      <c r="B10" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="30"/>
-    </row>
-    <row r="11" spans="1:4" s="22" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A11" s="40"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="40"/>
-    </row>
-    <row r="12" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A12" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A13" s="36"/>
-      <c r="B13" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A14" s="36"/>
-      <c r="B14" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A15" s="36"/>
-      <c r="B15" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A16" s="36"/>
-      <c r="B16" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A17" s="36"/>
-      <c r="B17" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A18" s="37"/>
-      <c r="B18" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="30"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A12:A18"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE7B6A0-3BBF-44A7-84C3-E6CD9C2928CA}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -4076,19 +4324,19 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A2" s="30"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="31"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="60.75" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="38" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="25" t="s">
         <v>242</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -4096,11 +4344,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A4" s="26"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="25" t="s">
         <v>244</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -4108,11 +4356,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A5" s="26"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="25" t="s">
         <v>246</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -4120,11 +4368,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="25" t="s">
         <v>248</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -4132,11 +4380,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A7" s="26"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="25" t="s">
         <v>250</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -4144,11 +4392,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A8" s="26"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="25" t="s">
         <v>252</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -4156,43 +4404,43 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="61.5" customHeight="1">
-      <c r="A9" s="26"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A10" s="26"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A11" s="34"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C11" s="31"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" s="29" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:4" s="23" customFormat="1" ht="47.25" customHeight="1">
+      <c r="A12" s="26"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="33"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="42" t="s">
         <v>223</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>255</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -4200,11 +4448,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A14" s="36"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="25" t="s">
         <v>257</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -4212,11 +4460,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="66.75" customHeight="1">
-      <c r="A15" s="36"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="25" t="s">
         <v>259</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -4224,11 +4472,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A16" s="36"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="25" t="s">
         <v>261</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -4236,11 +4484,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A17" s="36"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="25" t="s">
         <v>263</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -4248,11 +4496,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="47.25" customHeight="1">
-      <c r="A18" s="36"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="25" t="s">
         <v>265</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -4260,11 +4508,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="65.25" customHeight="1">
-      <c r="A19" s="36"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="25" t="s">
         <v>267</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -4272,19 +4520,19 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="61.5" customHeight="1">
-      <c r="A20" s="36"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C20" s="31"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="61.5" customHeight="1">
-      <c r="A21" s="37"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="31"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="3"/>
     </row>
   </sheetData>
@@ -4295,252 +4543,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9559937-0F27-4DE2-A20B-39F6C6177D47}">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="30.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="69.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A3" s="28"/>
-      <c r="B3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A8" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A9" s="24"/>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A10" s="24"/>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A11" s="24"/>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A13" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" customHeight="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A19" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A20" s="38"/>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30.75" customHeight="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A2:A6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>